<commit_message>
Included water dilution of pesticide
</commit_message>
<xml_diff>
--- a/Data/Iris_inputs.xlsx
+++ b/Data/Iris_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE42A0F-2C73-4A08-B413-3C9D66400435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844F4338-861B-43AA-89E3-143E21D9233F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <author>tc={B5C3BFB3-019D-426D-A008-79A436013E7A}</author>
   </authors>
   <commentList>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,7 +51,7 @@
     107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</t>
       </text>
     </comment>
-    <comment ref="C16" authorId="1" shapeId="0" xr:uid="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
+    <comment ref="C15" authorId="1" shapeId="0" xr:uid="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +59,7 @@
     190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</t>
       </text>
     </comment>
-    <comment ref="C17" authorId="2" shapeId="0" xr:uid="{7E0439F0-61E6-4462-942E-D17301560662}">
+    <comment ref="C16" authorId="2" shapeId="0" xr:uid="{7E0439F0-61E6-4462-942E-D17301560662}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -67,7 +67,7 @@
     750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</t>
       </text>
     </comment>
-    <comment ref="C37" authorId="3" shapeId="0" xr:uid="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
+    <comment ref="C36" authorId="3" shapeId="0" xr:uid="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -75,7 +75,7 @@
     80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</t>
       </text>
     </comment>
-    <comment ref="C38" authorId="4" shapeId="0" xr:uid="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
+    <comment ref="C37" authorId="4" shapeId="0" xr:uid="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -83,7 +83,7 @@
     80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</t>
       </text>
     </comment>
-    <comment ref="C39" authorId="5" shapeId="0" xr:uid="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
+    <comment ref="C38" authorId="5" shapeId="0" xr:uid="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -91,7 +91,7 @@
     64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</t>
       </text>
     </comment>
-    <comment ref="C40" authorId="6" shapeId="0" xr:uid="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
+    <comment ref="C39" authorId="6" shapeId="0" xr:uid="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="243">
   <si>
     <t>nominal</t>
   </si>
@@ -899,6 +899,12 @@
   </si>
   <si>
     <t>0,000q</t>
+  </si>
+  <si>
+    <t>dilution</t>
+  </si>
+  <si>
+    <t>ratio of water:pesticide</t>
   </si>
 </sst>
 </file>
@@ -1312,9 +1318,6 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1372,6 +1375,78 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1390,81 +1465,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,25 +1756,25 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C15" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
+  <threadedComment ref="C14" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{396ABCAF-54DB-4DB7-9877-C4D9CB0C752F}">
     <text>107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</text>
   </threadedComment>
-  <threadedComment ref="C16" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
+  <threadedComment ref="C15" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{DB4559B8-B4D5-46B7-9443-71ECDC1325D0}">
     <text>190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</text>
   </threadedComment>
-  <threadedComment ref="C17" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{7E0439F0-61E6-4462-942E-D17301560662}">
+  <threadedComment ref="C16" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{7E0439F0-61E6-4462-942E-D17301560662}">
     <text>750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</text>
   </threadedComment>
-  <threadedComment ref="C37" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
+  <threadedComment ref="C36" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{0DC24375-CA62-42B7-82D8-58C5246FFD6F}">
     <text>80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</text>
   </threadedComment>
-  <threadedComment ref="C38" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
+  <threadedComment ref="C37" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{72D2B639-7D47-4D26-A14C-D414C3B25E87}">
     <text>80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</text>
   </threadedComment>
-  <threadedComment ref="C39" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
+  <threadedComment ref="C38" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B1C3D0ED-7599-4C92-8848-AD9F3F4ACEF7}">
     <text>64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</text>
   </threadedComment>
-  <threadedComment ref="C40" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
+  <threadedComment ref="C39" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{B5C3BFB3-019D-426D-A008-79A436013E7A}">
     <text>0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</text>
   </threadedComment>
 </ThreadedComments>
@@ -1807,8 +1811,8 @@
   <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="3" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1826,14 +1830,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="87" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" s="33"/>
@@ -1867,7 +1871,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1891,7 +1895,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="96"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1915,11 +1919,11 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="96"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="77">
         <f>ROUNDUP((500/C7),0)</f>
         <v>953</v>
       </c>
@@ -1938,14 +1942,14 @@
         <v>158</v>
       </c>
       <c r="H6" s="50"/>
-      <c r="I6" s="81"/>
+      <c r="I6" s="80"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="96"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="77">
         <f>31.5/60</f>
         <v>0.52500000000000002</v>
       </c>
@@ -1964,14 +1968,14 @@
         <v>101</v>
       </c>
       <c r="H7" s="50"/>
-      <c r="I7" s="81"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="96"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="77">
         <v>380</v>
       </c>
       <c r="D8" s="11">
@@ -1988,12 +1992,12 @@
       <c r="G8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H8" s="60" t="s">
+      <c r="H8" s="59" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="96"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -2017,7 +2021,7 @@
       <c r="H9" s="55"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="96"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -2045,20 +2049,20 @@
       <c r="B11" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="84">
+      <c r="C11" s="83">
         <v>10</v>
       </c>
-      <c r="D11" s="84">
+      <c r="D11" s="83">
         <v>8</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="83">
         <v>12</v>
       </c>
       <c r="F11" s="41"/>
       <c r="G11" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="95" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2067,406 +2071,404 @@
       <c r="B12" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="84">
+      <c r="C12" s="83">
         <v>20</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="83">
         <v>16</v>
       </c>
-      <c r="E12" s="84">
+      <c r="E12" s="83">
         <v>24</v>
       </c>
       <c r="F12" s="41"/>
       <c r="G12" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="114"/>
+      <c r="H12" s="95"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="29"/>
       <c r="B13" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="84">
+      <c r="C13" s="83">
         <v>70</v>
       </c>
-      <c r="D13" s="84">
+      <c r="D13" s="83">
         <v>56</v>
       </c>
-      <c r="E13" s="84">
+      <c r="E13" s="83">
         <v>84</v>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="114"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="59"/>
-      <c r="B14" s="70" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" s="79">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="40">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="E14" s="40">
-        <f t="shared" ref="E14" si="2">1.2*C14</f>
-        <v>0.6</v>
-      </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="74" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="35" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A15" s="97" t="s">
+      <c r="H13" s="95"/>
+    </row>
+    <row r="14" spans="1:9" s="35" customFormat="1" ht="14.7" customHeight="1">
+      <c r="A14" s="102" t="s">
         <v>68</v>
       </c>
+      <c r="B14" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="48">
+        <f>214.17*$C$18</f>
+        <v>1499.1899999999998</v>
+      </c>
+      <c r="D14" s="48">
+        <f t="shared" si="0"/>
+        <v>1199.3519999999999</v>
+      </c>
+      <c r="E14" s="48">
+        <f t="shared" si="1"/>
+        <v>1799.0279999999998</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="74"/>
+    </row>
+    <row r="15" spans="1:9" s="35" customFormat="1">
+      <c r="A15" s="103"/>
       <c r="B15" s="47" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C15" s="48">
-        <f>214.17*$C$19</f>
-        <v>1499.1899999999998</v>
+        <f>0.38*$C$18</f>
+        <v>2.66</v>
       </c>
       <c r="D15" s="48">
         <f t="shared" si="0"/>
-        <v>1199.3519999999999</v>
+        <v>2.1280000000000001</v>
       </c>
       <c r="E15" s="48">
         <f t="shared" si="1"/>
-        <v>1799.0279999999998</v>
+        <v>3.1920000000000002</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G15" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="87" t="s">
-        <v>180</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="H15" s="111"/>
       <c r="I15" s="75"/>
     </row>
     <row r="16" spans="1:9" s="35" customFormat="1">
-      <c r="A16" s="98"/>
+      <c r="A16" s="103"/>
       <c r="B16" s="47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="48">
-        <f>0.38*$C$19</f>
-        <v>2.66</v>
+        <f>1.5*$C$18</f>
+        <v>10.5</v>
       </c>
       <c r="D16" s="48">
         <f t="shared" si="0"/>
-        <v>2.1280000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="E16" s="48">
         <f t="shared" si="1"/>
-        <v>3.1920000000000002</v>
+        <v>12.6</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>85</v>
       </c>
       <c r="G16" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="88"/>
-      <c r="I16" s="76"/>
-    </row>
-    <row r="17" spans="1:9" s="35" customFormat="1">
-      <c r="A17" s="98"/>
-      <c r="B17" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="48">
-        <f>1.5*$C$19</f>
-        <v>10.5</v>
-      </c>
-      <c r="D17" s="48">
-        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="H16" s="112"/>
+      <c r="I16" s="75"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="26">
+        <v>48</v>
+      </c>
+      <c r="D17" s="26">
+        <f t="shared" si="0"/>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="E17" s="26">
+        <f t="shared" si="1"/>
+        <v>57.599999999999994</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="1:13" ht="28.8">
+      <c r="A18" s="104"/>
+      <c r="B18" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="28">
+        <v>7</v>
+      </c>
+      <c r="D18" s="28">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="1"/>
         <v>8.4</v>
       </c>
-      <c r="E17" s="48">
-        <f t="shared" si="1"/>
-        <v>12.6</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" s="89"/>
-      <c r="I17" s="76"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="99" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="26">
-        <v>48</v>
-      </c>
-      <c r="D18" s="26">
-        <f t="shared" si="0"/>
-        <v>38.400000000000006</v>
-      </c>
-      <c r="E18" s="26">
-        <f t="shared" si="1"/>
-        <v>57.599999999999994</v>
-      </c>
       <c r="F18" s="27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="50"/>
-    </row>
-    <row r="19" spans="1:9" ht="28.8">
-      <c r="A19" s="99"/>
+        <v>77</v>
+      </c>
+      <c r="H18" s="76" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="104"/>
       <c r="B19" s="25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19" s="28">
-        <v>7</v>
+        <v>2250</v>
       </c>
       <c r="D19" s="28">
         <f t="shared" si="0"/>
-        <v>5.6000000000000005</v>
+        <v>1800</v>
       </c>
       <c r="E19" s="28">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>2700</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="77" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="99"/>
+        <v>82</v>
+      </c>
+      <c r="H19" s="50"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="104"/>
       <c r="B20" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" s="28">
-        <v>2250</v>
+        <v>10</v>
       </c>
       <c r="D20" s="28">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>8</v>
       </c>
       <c r="E20" s="28">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>12</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H20" s="50"/>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="99"/>
+    <row r="21" spans="1:13">
+      <c r="A21" s="104"/>
       <c r="B21" s="25" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C21" s="28">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D21" s="28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="E21" s="28">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>84</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H21" s="50"/>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="99"/>
+    <row r="22" spans="1:13">
+      <c r="A22" s="104"/>
       <c r="B22" s="25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="28">
-        <v>3</v>
+        <v>1E-4</v>
       </c>
       <c r="D22" s="28">
-        <f t="shared" si="0"/>
-        <v>2.4000000000000004</v>
+        <v>1E-4</v>
       </c>
       <c r="E22" s="28">
-        <f t="shared" si="1"/>
-        <v>3.5999999999999996</v>
+        <v>1E-4</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>84</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="99"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="104"/>
       <c r="B23" s="25" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C23" s="28">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="D23" s="28">
-        <v>1E-4</v>
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
       <c r="E23" s="28">
-        <v>1E-4</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="99"/>
-      <c r="B24" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="28">
-        <v>100</v>
-      </c>
-      <c r="D24" s="28">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="E24" s="28">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="27" t="s">
         <v>91</v>
       </c>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:13" ht="14.4" customHeight="1">
+      <c r="A24" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="12">
+        <v>63</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="0"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="E24" s="12">
+        <f t="shared" si="1"/>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="H24" s="50"/>
     </row>
-    <row r="25" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A25" s="100" t="s">
-        <v>45</v>
-      </c>
+    <row r="25" spans="1:13" ht="14.4" customHeight="1">
+      <c r="A25" s="106"/>
       <c r="B25" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" s="12">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D25" s="12">
         <f t="shared" si="0"/>
-        <v>50.400000000000006</v>
+        <v>24.8</v>
       </c>
       <c r="E25" s="12">
         <f t="shared" si="1"/>
-        <v>75.599999999999994</v>
+        <v>37.199999999999996</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H25" s="50"/>
     </row>
-    <row r="26" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A26" s="101"/>
+    <row r="26" spans="1:13">
+      <c r="A26" s="106"/>
       <c r="B26" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="12">
-        <v>31</v>
+        <v>1E-4</v>
       </c>
       <c r="D26" s="12">
-        <f t="shared" si="0"/>
-        <v>24.8</v>
+        <v>1E-4</v>
       </c>
       <c r="E26" s="12">
-        <f t="shared" si="1"/>
-        <v>37.199999999999996</v>
+        <v>1E-4</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H26" s="50"/>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="101"/>
+    <row r="27" spans="1:13">
+      <c r="A27" s="106"/>
       <c r="B27" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C27" s="12">
-        <v>1E-4</v>
+        <v>6</v>
       </c>
       <c r="D27" s="12">
-        <v>1E-4</v>
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
       </c>
       <c r="E27" s="12">
-        <v>1E-4</v>
+        <f t="shared" si="1"/>
+        <v>7.1999999999999993</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H27" s="50"/>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="101"/>
+    <row r="28" spans="1:13">
+      <c r="A28" s="106"/>
       <c r="B28" s="9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C28" s="12">
-        <v>6</v>
+        <v>1E-4</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000007</v>
+        <v>1E-4</v>
       </c>
       <c r="E28" s="12">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999993</v>
+        <v>1E-4</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" s="50"/>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="101"/>
+    <row r="29" spans="1:13">
+      <c r="A29" s="106"/>
       <c r="B29" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" s="12">
         <v>1E-4</v>
@@ -2479,34 +2481,38 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H29" s="50"/>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="101"/>
-      <c r="B30" s="9" t="s">
-        <v>15</v>
+    <row r="30" spans="1:13">
+      <c r="A30" s="106"/>
+      <c r="B30" s="36" t="s">
+        <v>16</v>
       </c>
       <c r="C30" s="12">
-        <v>1E-4</v>
-      </c>
-      <c r="D30" s="12">
-        <v>1E-4</v>
-      </c>
-      <c r="E30" s="12">
-        <v>1E-4</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30" s="50"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="101"/>
+        <v>1.25</v>
+      </c>
+      <c r="D30" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="106"/>
       <c r="B31" s="36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" s="12">
         <v>1.25</v>
@@ -2521,96 +2527,101 @@
       </c>
       <c r="F31" s="38"/>
       <c r="G31" s="38" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="H31" s="51" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="101"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="106"/>
       <c r="B32" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="12">
-        <v>1.25</v>
+        <v>18</v>
+      </c>
+      <c r="C32" s="70">
+        <v>1</v>
       </c>
       <c r="D32" s="37">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E32" s="37">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="H32" s="51" t="s">
-        <v>237</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="H32" s="113" t="s">
+        <v>179</v>
+      </c>
+      <c r="K32" s="86" t="s">
+        <v>213</v>
+      </c>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="101"/>
+      <c r="A33" s="106"/>
       <c r="B33" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="71">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C33" s="70">
+        <v>1.2</v>
       </c>
       <c r="D33" s="37">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.96</v>
       </c>
       <c r="E33" s="37">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.44</v>
       </c>
       <c r="F33" s="38"/>
       <c r="G33" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="H33" s="90" t="s">
-        <v>179</v>
-      </c>
-      <c r="K33" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="L33" s="105"/>
-      <c r="M33" s="105"/>
+        <v>115</v>
+      </c>
+      <c r="H33" s="114"/>
+      <c r="K33" s="96" t="s">
+        <v>216</v>
+      </c>
+      <c r="L33" s="96"/>
+      <c r="M33" s="96"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="101"/>
+      <c r="A34" s="106"/>
       <c r="B34" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="71">
-        <v>1.2</v>
+        <v>19</v>
+      </c>
+      <c r="C34" s="70">
+        <v>1</v>
       </c>
       <c r="D34" s="37">
-        <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="E34" s="37">
-        <f t="shared" si="1"/>
-        <v>1.44</v>
+        <v>1</v>
       </c>
       <c r="F34" s="38"/>
       <c r="G34" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="H34" s="91"/>
-      <c r="K34" s="115" t="s">
-        <v>216</v>
-      </c>
-      <c r="L34" s="115"/>
-      <c r="M34" s="115"/>
+        <v>116</v>
+      </c>
+      <c r="H34" s="114"/>
+      <c r="K34" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="L34" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="M34" s="50" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="101"/>
+      <c r="A35" s="106"/>
       <c r="B35" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="71">
+        <v>20</v>
+      </c>
+      <c r="C35" s="70">
         <v>1</v>
       </c>
       <c r="D35" s="37">
@@ -2621,842 +2632,835 @@
       </c>
       <c r="F35" s="38"/>
       <c r="G35" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="91"/>
-      <c r="K35" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="H35" s="115"/>
+      <c r="K35" s="50">
+        <v>0.33</v>
+      </c>
+      <c r="L35" s="50">
+        <v>8000</v>
+      </c>
+      <c r="M35" s="50">
+        <f>L35*K35</f>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="14.4" customHeight="1">
+      <c r="A36" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="53">
+        <f>4.44*$C$19</f>
+        <v>9990</v>
+      </c>
+      <c r="D36" s="53">
+        <f t="shared" si="0"/>
+        <v>7992</v>
+      </c>
+      <c r="E36" s="53">
+        <f t="shared" si="1"/>
+        <v>11988</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H36" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36" s="75"/>
+      <c r="K36" s="96" t="s">
+        <v>215</v>
+      </c>
+      <c r="L36" s="96"/>
+      <c r="M36" s="96"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="93"/>
+      <c r="B37" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="53">
+        <f>0.00444*$C$19</f>
+        <v>9.99</v>
+      </c>
+      <c r="D37" s="53">
+        <f t="shared" si="0"/>
+        <v>7.9920000000000009</v>
+      </c>
+      <c r="E37" s="53">
+        <f t="shared" si="1"/>
+        <v>11.988</v>
+      </c>
+      <c r="F37" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="114"/>
+      <c r="I37" s="75"/>
+      <c r="K37" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="L35" s="50" t="s">
+      <c r="L37" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="M35" s="50" t="s">
+      <c r="M37" s="50" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="101"/>
-      <c r="B36" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="71">
-        <v>1</v>
-      </c>
-      <c r="D36" s="37">
-        <v>1</v>
-      </c>
-      <c r="E36" s="37">
-        <v>1</v>
-      </c>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="H36" s="92"/>
-      <c r="K36" s="50">
-        <v>0.33</v>
-      </c>
-      <c r="L36" s="50">
-        <v>8000</v>
-      </c>
-      <c r="M36" s="50">
-        <f>L36*K36</f>
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A37" s="111" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="53">
-        <f>4.44*$C$20</f>
-        <v>9990</v>
-      </c>
-      <c r="D37" s="53">
-        <f t="shared" si="0"/>
-        <v>7992</v>
-      </c>
-      <c r="E37" s="53">
-        <f t="shared" si="1"/>
-        <v>11988</v>
-      </c>
-      <c r="F37" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="G37" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="H37" s="90" t="s">
-        <v>182</v>
-      </c>
-      <c r="I37" s="76"/>
-      <c r="K37" s="115" t="s">
-        <v>215</v>
-      </c>
-      <c r="L37" s="115"/>
-      <c r="M37" s="115"/>
-    </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="112"/>
+      <c r="A38" s="93"/>
       <c r="B38" s="52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38" s="53">
-        <f>0.00444*$C$20</f>
-        <v>9.99</v>
+        <f>0.00356*$C$19</f>
+        <v>8.01</v>
       </c>
       <c r="D38" s="53">
         <f t="shared" si="0"/>
-        <v>7.9920000000000009</v>
+        <v>6.4080000000000004</v>
       </c>
       <c r="E38" s="53">
         <f t="shared" si="1"/>
-        <v>11.988</v>
+        <v>9.6120000000000001</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>85</v>
       </c>
       <c r="G38" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="H38" s="91"/>
-      <c r="I38" s="76"/>
-      <c r="K38" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="L38" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="M38" s="50" t="s">
-        <v>212</v>
+        <v>120</v>
+      </c>
+      <c r="H38" s="114"/>
+      <c r="I38" s="75"/>
+      <c r="K38" s="65">
+        <v>0.33</v>
+      </c>
+      <c r="L38" s="50">
+        <v>1500</v>
+      </c>
+      <c r="M38" s="97">
+        <f>L38*K38+K39*L39+K40*L40</f>
+        <v>2805</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="112"/>
+      <c r="A39" s="93"/>
       <c r="B39" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C39" s="53">
-        <f>0.00356*$C$20</f>
-        <v>8.01</v>
+        <f>0.000015*$C$19</f>
+        <v>3.3750000000000002E-2</v>
       </c>
       <c r="D39" s="53">
         <f t="shared" si="0"/>
-        <v>6.4080000000000004</v>
+        <v>2.7000000000000003E-2</v>
       </c>
       <c r="E39" s="53">
         <f t="shared" si="1"/>
-        <v>9.6120000000000001</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>85</v>
       </c>
       <c r="G39" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="H39" s="91"/>
-      <c r="I39" s="76"/>
-      <c r="K39" s="66">
+        <v>121</v>
+      </c>
+      <c r="H39" s="115"/>
+      <c r="I39" s="75"/>
+      <c r="K39" s="65">
         <v>0.33</v>
       </c>
       <c r="L39" s="50">
-        <v>1500</v>
-      </c>
-      <c r="M39" s="116">
-        <f>L39*K39+K40*L40+K41*L41</f>
-        <v>2805</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="M39" s="97"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="112"/>
-      <c r="B40" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="53">
-        <f>0.000015*$C$20</f>
-        <v>3.3750000000000002E-2</v>
-      </c>
-      <c r="D40" s="53">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000003E-2</v>
-      </c>
-      <c r="E40" s="53">
-        <f t="shared" si="1"/>
-        <v>4.0500000000000001E-2</v>
-      </c>
-      <c r="F40" s="54" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="H40" s="92"/>
-      <c r="I40" s="76"/>
-      <c r="K40" s="66">
+      <c r="A40" s="94"/>
+      <c r="B40" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E40" s="15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="50"/>
+      <c r="K40" s="65">
         <v>0.33</v>
       </c>
       <c r="L40" s="50">
-        <v>6500</v>
-      </c>
-      <c r="M40" s="116"/>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="113"/>
-      <c r="B41" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="15">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D41" s="15">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E41" s="15">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="H41" s="50"/>
-      <c r="K41" s="66">
-        <v>0.33</v>
-      </c>
-      <c r="L41" s="50">
         <v>500</v>
       </c>
-      <c r="M41" s="116"/>
-    </row>
-    <row r="42" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A42" s="108" t="s">
+      <c r="M40" s="97"/>
+    </row>
+    <row r="41" spans="1:14" ht="14.4" customHeight="1">
+      <c r="A41" s="89" t="s">
         <v>47</v>
       </c>
+      <c r="B41" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="18">
+        <v>330</v>
+      </c>
+      <c r="D41" s="18">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="E41" s="18">
+        <f t="shared" si="1"/>
+        <v>396</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H41" s="50" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="90"/>
       <c r="B42" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C42" s="18">
-        <v>330</v>
+        <v>1E-4</v>
       </c>
       <c r="D42" s="18">
-        <f t="shared" si="0"/>
-        <v>264</v>
+        <v>1E-4</v>
       </c>
       <c r="E42" s="18">
-        <f t="shared" si="1"/>
-        <v>396</v>
+        <v>1E-4</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>7</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H42" s="50" t="s">
-        <v>218</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="H42" s="50"/>
+      <c r="K42" s="96" t="s">
+        <v>198</v>
+      </c>
+      <c r="L42" s="96"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="109"/>
+      <c r="A43" s="90"/>
       <c r="B43" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C43" s="18">
-        <v>1E-4</v>
+        <v>2805</v>
       </c>
       <c r="D43" s="18">
-        <v>1E-4</v>
+        <f t="shared" si="0"/>
+        <v>2244</v>
       </c>
       <c r="E43" s="18">
-        <v>1E-4</v>
+        <f t="shared" si="1"/>
+        <v>3366</v>
       </c>
       <c r="F43" s="19" t="s">
         <v>7</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="H43" s="50"/>
-      <c r="K43" s="115" t="s">
-        <v>198</v>
-      </c>
-      <c r="L43" s="115"/>
+        <v>124</v>
+      </c>
+      <c r="H43" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="K43" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="L43" s="50">
+        <v>116</v>
+      </c>
+      <c r="M43" s="65">
+        <f>L43/SUM($L$43:$L$45)</f>
+        <v>0.30526315789473685</v>
+      </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="109"/>
+      <c r="A44" s="90"/>
       <c r="B44" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C44" s="18">
-        <v>2805</v>
+        <v>0.03</v>
       </c>
       <c r="D44" s="18">
         <f t="shared" si="0"/>
-        <v>2244</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E44" s="18">
         <f t="shared" si="1"/>
-        <v>3366</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="H44" s="50" t="s">
-        <v>217</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="H44" s="50"/>
       <c r="K44" s="50" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L44" s="50">
-        <v>116</v>
-      </c>
-      <c r="M44" s="66">
-        <f>L44/SUM($L$44:$L$46)</f>
-        <v>0.30526315789473685</v>
+        <f>184+56</f>
+        <v>240</v>
+      </c>
+      <c r="M44" s="65">
+        <f t="shared" ref="M44:M45" si="2">L44/SUM($L$43:$L$45)</f>
+        <v>0.63157894736842102</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="109"/>
+      <c r="A45" s="90"/>
       <c r="B45" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C45" s="18">
-        <v>0.03</v>
+        <v>1E-4</v>
       </c>
       <c r="D45" s="18">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="E45" s="18">
-        <f t="shared" si="1"/>
-        <v>3.5999999999999997E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="F45" s="19" t="s">
         <v>38</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H45" s="50"/>
       <c r="K45" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L45" s="50">
-        <f>184+56</f>
-        <v>240</v>
-      </c>
-      <c r="M45" s="66">
-        <f t="shared" ref="M45:M46" si="3">L45/SUM($L$44:$L$46)</f>
-        <v>0.63157894736842102</v>
+        <f>0.1*L44</f>
+        <v>24</v>
+      </c>
+      <c r="M45" s="65">
+        <f t="shared" si="2"/>
+        <v>6.3157894736842107E-2</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="109"/>
+      <c r="A46" s="90"/>
       <c r="B46" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C46" s="18">
-        <v>1E-4</v>
+        <v>2.44</v>
       </c>
       <c r="D46" s="18">
-        <v>1E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.952</v>
       </c>
       <c r="E46" s="18">
-        <v>1E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.9279999999999999</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>38</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H46" s="50"/>
-      <c r="K46" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="L46" s="50">
-        <f>0.1*L45</f>
-        <v>24</v>
-      </c>
-      <c r="M46" s="66">
-        <f t="shared" si="3"/>
-        <v>6.3157894736842107E-2</v>
-      </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="109"/>
+      <c r="A47" s="91"/>
       <c r="B47" s="17" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="C47" s="18">
-        <v>2.44</v>
+        <v>2805</v>
       </c>
       <c r="D47" s="18">
         <f t="shared" si="0"/>
-        <v>1.952</v>
+        <v>2244</v>
       </c>
       <c r="E47" s="18">
         <f t="shared" si="1"/>
-        <v>2.9279999999999999</v>
+        <v>3366</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="H47" s="50"/>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" s="110"/>
-      <c r="B48" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C48" s="18">
-        <v>2805</v>
-      </c>
-      <c r="D48" s="18">
-        <f t="shared" si="0"/>
-        <v>2244</v>
-      </c>
-      <c r="E48" s="18">
-        <f t="shared" si="1"/>
-        <v>3366</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="H48" s="50"/>
-      <c r="K48" s="115" t="s">
+      <c r="K47" s="96" t="s">
         <v>199</v>
       </c>
-      <c r="L48" s="115"/>
-      <c r="M48" s="115"/>
-      <c r="N48" s="115"/>
-    </row>
-    <row r="49" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A49" s="102" t="s">
+      <c r="L47" s="96"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="96"/>
+    </row>
+    <row r="48" spans="1:14" ht="14.4" customHeight="1">
+      <c r="A48" s="107" t="s">
         <v>44</v>
       </c>
+      <c r="B48" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="C48" s="32">
+        <f>34.5/C53</f>
+        <v>3.9115646258503403E-2</v>
+      </c>
+      <c r="D48" s="30">
+        <f t="shared" si="0"/>
+        <v>3.1292517006802724E-2</v>
+      </c>
+      <c r="E48" s="30">
+        <f t="shared" si="1"/>
+        <v>4.6938775510204082E-2</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H48" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="I48" s="79"/>
+      <c r="K48" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="L48" s="64">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="108"/>
       <c r="B49" s="20" t="s">
-        <v>228</v>
+        <v>171</v>
       </c>
       <c r="C49" s="32">
-        <f>34.5/C54</f>
-        <v>3.9115646258503403E-2</v>
-      </c>
-      <c r="D49" s="30">
-        <f t="shared" si="0"/>
-        <v>3.1292517006802724E-2</v>
-      </c>
-      <c r="E49" s="30">
-        <f t="shared" si="1"/>
-        <v>4.6938775510204082E-2</v>
+        <f>23/C54</f>
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="D49" s="21">
+        <f t="shared" si="0"/>
+        <v>0.6133333333333334</v>
+      </c>
+      <c r="E49" s="21">
+        <f t="shared" si="1"/>
+        <v>0.92</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="H49" s="90" t="s">
-        <v>183</v>
-      </c>
-      <c r="I49" s="80"/>
-      <c r="K49" s="64" t="s">
-        <v>193</v>
-      </c>
-      <c r="L49" s="65">
-        <v>418</v>
+        <v>132</v>
+      </c>
+      <c r="H49" s="114"/>
+      <c r="I49" s="79"/>
+      <c r="K49" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="L49" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="M49" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="N49" s="50" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="103"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="C50" s="32">
-        <f>23/C55</f>
-        <v>0.76666666666666672</v>
+        <v>173</v>
+      </c>
+      <c r="C50" s="82">
+        <f>9/C55</f>
+        <v>0.15</v>
       </c>
       <c r="D50" s="21">
-        <f t="shared" si="0"/>
-        <v>0.6133333333333334</v>
+        <f>0.8*C50</f>
+        <v>0.12</v>
       </c>
       <c r="E50" s="21">
         <f t="shared" si="1"/>
-        <v>0.92</v>
+        <v>0.18</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="91"/>
-      <c r="I50" s="80"/>
-      <c r="K50" s="62" t="s">
-        <v>189</v>
-      </c>
-      <c r="L50" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="M50" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="N50" s="50" t="s">
-        <v>191</v>
+        <v>177</v>
+      </c>
+      <c r="H50" s="114"/>
+      <c r="I50" s="79"/>
+      <c r="K50" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="L50" s="65">
+        <v>0.9</v>
+      </c>
+      <c r="M50" s="50">
+        <f>5/5</f>
+        <v>1</v>
+      </c>
+      <c r="N50" s="62">
+        <f>M50/$L$48</f>
+        <v>2.3923444976076554E-3</v>
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="103"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C51" s="83">
-        <f>9/C56</f>
-        <v>0.15</v>
+        <v>225</v>
+      </c>
+      <c r="C51" s="32">
+        <f>9.5/C56</f>
+        <v>0.15305300467214436</v>
       </c>
       <c r="D51" s="21">
         <f>0.8*C51</f>
-        <v>0.12</v>
+        <v>0.12244240373771549</v>
       </c>
       <c r="E51" s="21">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
+        <f t="shared" ref="E51" si="3">1.2*C51</f>
+        <v>0.18366360560657322</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="H51" s="91"/>
-      <c r="I51" s="80"/>
-      <c r="K51" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="L51" s="66">
-        <v>0.9</v>
-      </c>
-      <c r="M51" s="50">
-        <f>5/5</f>
-        <v>1</v>
-      </c>
-      <c r="N51" s="63">
-        <f>M51/$L$49</f>
-        <v>2.3923444976076554E-3</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="H51" s="114"/>
+      <c r="I51" s="79"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="65"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="62"/>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="103"/>
+      <c r="A52" s="108"/>
       <c r="B52" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="C52" s="32">
-        <f>9.5/C57</f>
-        <v>0.15305300467214436</v>
+        <v>224</v>
+      </c>
+      <c r="C52" s="82">
+        <f>9/C57</f>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D52" s="21">
-        <f>0.8*C52</f>
-        <v>0.12244240373771549</v>
+        <f t="shared" si="0"/>
+        <v>1.2E-2</v>
       </c>
       <c r="E52" s="21">
-        <f t="shared" ref="E52" si="4">1.2*C52</f>
-        <v>0.18366360560657322</v>
+        <f t="shared" si="1"/>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="H52" s="91"/>
-      <c r="I52" s="80"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="66"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="63"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="103"/>
-      <c r="B53" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="C53" s="83">
-        <f>9/C58</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D53" s="21">
-        <f t="shared" si="0"/>
-        <v>1.2E-2</v>
-      </c>
-      <c r="E53" s="21">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="H53" s="91"/>
-      <c r="I53" s="80"/>
-      <c r="K53" s="50" t="s">
+      <c r="H52" s="114"/>
+      <c r="I52" s="79"/>
+      <c r="K52" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="L53" s="66">
+      <c r="L52" s="65">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M53" s="50">
+      <c r="M52" s="50">
         <f>29/5</f>
         <v>5.8</v>
       </c>
-      <c r="N53" s="63">
-        <f>M53/$L$49</f>
+      <c r="N52" s="62">
+        <f>M52/$L$48</f>
         <v>1.3875598086124402E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="103"/>
-      <c r="B54" s="20" t="s">
+    <row r="53" spans="1:14">
+      <c r="A53" s="108"/>
+      <c r="B53" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="C54" s="83">
+      <c r="C53" s="82">
         <f>14.7*60</f>
         <v>882</v>
       </c>
+      <c r="D53" s="21">
+        <f t="shared" si="0"/>
+        <v>705.6</v>
+      </c>
+      <c r="E53" s="21">
+        <f t="shared" si="1"/>
+        <v>1058.3999999999999</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="H53" s="114"/>
+      <c r="I53" s="79"/>
+      <c r="K53" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="L53" s="65">
+        <v>0.3</v>
+      </c>
+      <c r="M53" s="50">
+        <f>13/5</f>
+        <v>2.6</v>
+      </c>
+      <c r="N53" s="62">
+        <f>M53/$L$48</f>
+        <v>6.2200956937799043E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="108"/>
+      <c r="B54" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="82">
+        <v>30</v>
+      </c>
       <c r="D54" s="21">
         <f t="shared" si="0"/>
-        <v>705.6</v>
+        <v>24</v>
       </c>
       <c r="E54" s="21">
         <f t="shared" si="1"/>
-        <v>1058.3999999999999</v>
+        <v>36</v>
       </c>
       <c r="F54" s="22" t="s">
         <v>175</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="H54" s="91"/>
-      <c r="I54" s="80"/>
-      <c r="K54" s="50" t="s">
-        <v>200</v>
-      </c>
-      <c r="L54" s="66">
-        <v>0.3</v>
-      </c>
-      <c r="M54" s="50">
-        <f>13/5</f>
-        <v>2.6</v>
-      </c>
-      <c r="N54" s="63">
-        <f>M54/$L$49</f>
-        <v>6.2200956937799043E-3</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H54" s="114"/>
+      <c r="I54" s="79"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="103"/>
+      <c r="A55" s="108"/>
       <c r="B55" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="C55" s="83">
-        <v>30</v>
+        <v>174</v>
+      </c>
+      <c r="C55" s="82">
+        <v>60</v>
       </c>
       <c r="D55" s="21">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E55" s="21">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F55" s="22" t="s">
         <v>175</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="H55" s="91"/>
-      <c r="I55" s="80"/>
+        <v>176</v>
+      </c>
+      <c r="H55" s="114"/>
+      <c r="I55" s="79"/>
+      <c r="K55" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="L55" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="M55" s="50" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="103"/>
-      <c r="B56" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="C56" s="83">
-        <v>60</v>
+      <c r="A56" s="108"/>
+      <c r="B56" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" s="82">
+        <f>60*1.0345</f>
+        <v>62.07</v>
       </c>
       <c r="D56" s="21">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>49.656000000000006</v>
       </c>
       <c r="E56" s="21">
-        <f t="shared" si="1"/>
-        <v>72</v>
+        <f t="shared" ref="E56" si="4">1.2*C56</f>
+        <v>74.483999999999995</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>175</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="H56" s="91"/>
-      <c r="I56" s="80"/>
+        <v>223</v>
+      </c>
+      <c r="H56" s="114"/>
+      <c r="I56" s="79"/>
       <c r="K56" s="50" t="s">
-        <v>204</v>
-      </c>
-      <c r="L56" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="M56" s="50" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="L56" s="66">
+        <v>40</v>
+      </c>
+      <c r="M56" s="50">
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="103"/>
+      <c r="A57" s="108"/>
       <c r="B57" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C57" s="83">
-        <f>60*1.0345</f>
-        <v>62.07</v>
+        <v>221</v>
+      </c>
+      <c r="C57" s="82">
+        <v>600</v>
       </c>
       <c r="D57" s="21">
         <f t="shared" si="0"/>
-        <v>49.656000000000006</v>
+        <v>480</v>
       </c>
       <c r="E57" s="21">
-        <f t="shared" ref="E57" si="5">1.2*C57</f>
-        <v>74.483999999999995</v>
+        <f t="shared" si="1"/>
+        <v>720</v>
       </c>
       <c r="F57" s="22" t="s">
         <v>175</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="H57" s="91"/>
-      <c r="I57" s="80"/>
-      <c r="K57" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="L57" s="67">
-        <v>40</v>
+        <v>222</v>
+      </c>
+      <c r="H57" s="115"/>
+      <c r="I57" s="79"/>
+      <c r="K57" s="68" t="s">
+        <v>194</v>
+      </c>
+      <c r="L57" s="66">
+        <v>12</v>
       </c>
       <c r="M57" s="50">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="103"/>
+      <c r="A58" s="108"/>
       <c r="B58" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="C58" s="83">
-        <v>600</v>
+        <v>163</v>
+      </c>
+      <c r="C58" s="32">
+        <v>4.3</v>
       </c>
       <c r="D58" s="21">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>3.44</v>
       </c>
       <c r="E58" s="21">
         <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>175</v>
+        <v>5.1599999999999993</v>
+      </c>
+      <c r="F58" s="24" t="s">
+        <v>169</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="H58" s="92"/>
-      <c r="I58" s="80"/>
-      <c r="K58" s="69" t="s">
-        <v>194</v>
-      </c>
-      <c r="L58" s="67">
-        <v>12</v>
+        <v>168</v>
+      </c>
+      <c r="H58" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="K58" s="68" t="s">
+        <v>209</v>
+      </c>
+      <c r="L58" s="66">
+        <v>0.5</v>
       </c>
       <c r="M58" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="108"/>
+      <c r="B59" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="32">
+        <v>0.81</v>
+      </c>
+      <c r="D59" s="21">
+        <f t="shared" si="0"/>
+        <v>0.64800000000000013</v>
+      </c>
+      <c r="E59" s="21">
+        <f t="shared" si="1"/>
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F59" s="24"/>
+      <c r="G59" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="H59" s="81" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="108"/>
+      <c r="B60" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="32">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59" s="103"/>
-      <c r="B59" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" s="32">
-        <v>4.3</v>
-      </c>
-      <c r="D59" s="21">
-        <f t="shared" si="0"/>
-        <v>3.44</v>
-      </c>
-      <c r="E59" s="21">
-        <f t="shared" si="1"/>
-        <v>5.1599999999999993</v>
-      </c>
-      <c r="F59" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="G59" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H59" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="K59" s="69" t="s">
-        <v>209</v>
-      </c>
-      <c r="L59" s="67">
-        <v>0.5</v>
-      </c>
-      <c r="M59" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" s="103"/>
-      <c r="B60" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" s="32">
-        <v>0.81</v>
-      </c>
       <c r="D60" s="21">
         <f t="shared" si="0"/>
-        <v>0.64800000000000013</v>
+        <v>1.6</v>
       </c>
       <c r="E60" s="21">
         <f t="shared" si="1"/>
-        <v>0.97199999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="H60" s="82" t="s">
-        <v>235</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="H60" s="117"/>
     </row>
     <row r="61" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A61" s="103"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="42" t="s">
         <v>41</v>
       </c>
@@ -3478,7 +3482,7 @@
       <c r="G61" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="H61" s="90" t="s">
+      <c r="H61" s="113" t="s">
         <v>185</v>
       </c>
       <c r="I61" t="s">
@@ -3487,13 +3491,13 @@
       <c r="K61" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="L61" s="68">
-        <f>N51*L51*L44 + L57/M57</f>
+      <c r="L61" s="67">
+        <f>N50*L50*L43 + L56/M56</f>
         <v>4.2497607655502394</v>
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="103"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="42" t="s">
         <v>42</v>
       </c>
@@ -3515,17 +3519,17 @@
       <c r="G62" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="H62" s="91"/>
+      <c r="H62" s="114"/>
       <c r="K62" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="L62" s="68">
-        <f>N53*L53*L45 +L59</f>
+      <c r="L62" s="67">
+        <f>N52*L52*L44 +L58</f>
         <v>2.3315789473684214</v>
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="103"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="42" t="s">
         <v>92</v>
       </c>
@@ -3547,18 +3551,18 @@
       <c r="G63" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="H63" s="91"/>
+      <c r="H63" s="114"/>
       <c r="K63" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="L63" s="68">
-        <f>N54*L54*L46</f>
+      <c r="L63" s="67">
+        <f>N53*L53*L45</f>
         <v>4.4784688995215309E-2</v>
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="104"/>
-      <c r="B64" s="73" t="s">
+      <c r="A64" s="109"/>
+      <c r="B64" s="72" t="s">
         <v>93</v>
       </c>
       <c r="C64" s="43">
@@ -3579,384 +3583,384 @@
       <c r="G64" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="H64" s="92"/>
-      <c r="K64" s="62" t="s">
+      <c r="H64" s="115"/>
+      <c r="K64" s="61" t="s">
         <v>208</v>
       </c>
       <c r="L64" s="50">
-        <f>L58/M58</f>
+        <f>L57/M57</f>
         <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A65" s="93" t="s">
+      <c r="A65" s="98" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="85">
+      <c r="C65" s="84">
         <v>0.25</v>
       </c>
-      <c r="D65" s="85">
+      <c r="D65" s="84">
         <v>0.2</v>
       </c>
-      <c r="E65" s="85">
+      <c r="E65" s="84">
         <v>0.3</v>
       </c>
       <c r="F65" s="58"/>
       <c r="G65" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="H65" s="87" t="s">
+      <c r="H65" s="110" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="94"/>
+      <c r="A66" s="99"/>
       <c r="B66" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="85">
+      <c r="C66" s="84">
         <v>0.2</v>
       </c>
-      <c r="D66" s="85">
+      <c r="D66" s="84">
         <v>0.16000000000000003</v>
       </c>
-      <c r="E66" s="85">
+      <c r="E66" s="84">
         <v>0.24</v>
       </c>
       <c r="F66" s="58"/>
       <c r="G66" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="H66" s="88"/>
+      <c r="H66" s="111"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="94"/>
+      <c r="A67" s="99"/>
       <c r="B67" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C67" s="85">
+      <c r="C67" s="84">
         <v>0.2</v>
       </c>
-      <c r="D67" s="85">
+      <c r="D67" s="84">
         <v>0.16000000000000003</v>
       </c>
-      <c r="E67" s="85">
+      <c r="E67" s="84">
         <v>0.24</v>
       </c>
       <c r="F67" s="58"/>
       <c r="G67" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="H67" s="88"/>
+      <c r="H67" s="111"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="94"/>
+      <c r="A68" s="99"/>
       <c r="B68" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="86">
+      <c r="C68" s="85">
         <v>0.2</v>
       </c>
-      <c r="D68" s="85">
+      <c r="D68" s="84">
         <v>0.16000000000000003</v>
       </c>
-      <c r="E68" s="85">
+      <c r="E68" s="84">
         <v>0.24</v>
       </c>
       <c r="F68" s="58"/>
       <c r="G68" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="H68" s="88"/>
+      <c r="H68" s="111"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="94"/>
+      <c r="A69" s="99"/>
       <c r="B69" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="86">
+      <c r="C69" s="85">
         <v>0.5</v>
       </c>
-      <c r="D69" s="85">
+      <c r="D69" s="84">
         <v>0.4</v>
       </c>
-      <c r="E69" s="85">
+      <c r="E69" s="84">
         <v>0.6</v>
       </c>
       <c r="F69" s="58"/>
       <c r="G69" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="H69" s="88"/>
+      <c r="H69" s="111"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="94"/>
+      <c r="A70" s="99"/>
       <c r="B70" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="86">
+      <c r="C70" s="85">
         <v>0.5</v>
       </c>
-      <c r="D70" s="85">
+      <c r="D70" s="84">
         <v>0.4</v>
       </c>
-      <c r="E70" s="85">
+      <c r="E70" s="84">
         <v>0.6</v>
       </c>
       <c r="F70" s="58"/>
       <c r="G70" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="88"/>
+      <c r="H70" s="111"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="94"/>
+      <c r="A71" s="99"/>
       <c r="B71" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C71" s="86">
+      <c r="C71" s="85">
         <v>0.25</v>
       </c>
-      <c r="D71" s="85">
+      <c r="D71" s="84">
         <v>0.2</v>
       </c>
-      <c r="E71" s="85">
+      <c r="E71" s="84">
         <v>0.3</v>
       </c>
       <c r="F71" s="58"/>
       <c r="G71" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="H71" s="88"/>
+      <c r="H71" s="111"/>
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="94"/>
+      <c r="A72" s="99"/>
       <c r="B72" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="86">
+      <c r="C72" s="85">
         <v>0.1</v>
       </c>
-      <c r="D72" s="85">
+      <c r="D72" s="84">
         <v>8.0000000000000016E-2</v>
       </c>
-      <c r="E72" s="85">
+      <c r="E72" s="84">
         <v>0.12</v>
       </c>
       <c r="F72" s="58"/>
       <c r="G72" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="H72" s="88"/>
+      <c r="H72" s="111"/>
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="94"/>
+      <c r="A73" s="99"/>
       <c r="B73" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C73" s="86">
+      <c r="C73" s="85">
         <v>0.1</v>
       </c>
-      <c r="D73" s="85">
+      <c r="D73" s="84">
         <v>8.0000000000000016E-2</v>
       </c>
-      <c r="E73" s="85">
+      <c r="E73" s="84">
         <v>0.12</v>
       </c>
       <c r="F73" s="58"/>
       <c r="G73" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="H73" s="88"/>
+      <c r="H73" s="111"/>
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="94"/>
+      <c r="A74" s="99"/>
       <c r="B74" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C74" s="86">
+      <c r="C74" s="85">
         <v>0.1</v>
       </c>
-      <c r="D74" s="85">
+      <c r="D74" s="84">
         <v>8.0000000000000016E-2</v>
       </c>
-      <c r="E74" s="85">
+      <c r="E74" s="84">
         <v>0.12</v>
       </c>
       <c r="F74" s="58"/>
       <c r="G74" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H74" s="88"/>
+      <c r="H74" s="111"/>
       <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="94"/>
+      <c r="A75" s="99"/>
       <c r="B75" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="86">
+      <c r="C75" s="85">
         <v>0.45</v>
       </c>
-      <c r="D75" s="85">
+      <c r="D75" s="84">
         <v>0.36000000000000004</v>
       </c>
-      <c r="E75" s="85">
+      <c r="E75" s="84">
         <v>0.54</v>
       </c>
       <c r="F75" s="58"/>
       <c r="G75" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="H75" s="88"/>
+      <c r="H75" s="111"/>
       <c r="K75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="94"/>
+      <c r="A76" s="99"/>
       <c r="B76" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C76" s="86">
+      <c r="C76" s="85">
         <v>0.45</v>
       </c>
-      <c r="D76" s="85">
+      <c r="D76" s="84">
         <v>0.36000000000000004</v>
       </c>
-      <c r="E76" s="85">
+      <c r="E76" s="84">
         <v>0.54</v>
       </c>
       <c r="F76" s="58"/>
       <c r="G76" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="H76" s="88"/>
+      <c r="H76" s="111"/>
       <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="94"/>
+      <c r="A77" s="99"/>
       <c r="B77" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C77" s="86">
+      <c r="C77" s="85">
         <v>0.5</v>
       </c>
-      <c r="D77" s="85">
+      <c r="D77" s="84">
         <v>0.4</v>
       </c>
-      <c r="E77" s="85">
+      <c r="E77" s="84">
         <v>0.6</v>
       </c>
       <c r="F77" s="58"/>
       <c r="G77" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="H77" s="88"/>
+      <c r="H77" s="111"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="94"/>
+      <c r="A78" s="99"/>
       <c r="B78" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C78" s="85">
+      <c r="C78" s="84">
         <v>0.7</v>
       </c>
-      <c r="D78" s="85">
+      <c r="D78" s="84">
         <v>0.55999999999999994</v>
       </c>
-      <c r="E78" s="85">
+      <c r="E78" s="84">
         <v>0.84</v>
       </c>
       <c r="F78" s="58"/>
       <c r="G78" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="H78" s="88"/>
+      <c r="H78" s="111"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="94"/>
+      <c r="A79" s="99"/>
       <c r="B79" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C79" s="85">
+      <c r="C79" s="84">
         <v>0.7</v>
       </c>
-      <c r="D79" s="85">
+      <c r="D79" s="84">
         <v>0.55999999999999994</v>
       </c>
-      <c r="E79" s="85">
+      <c r="E79" s="84">
         <v>0.84</v>
       </c>
       <c r="F79" s="58"/>
       <c r="G79" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H79" s="88"/>
+      <c r="H79" s="111"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="94"/>
+      <c r="A80" s="99"/>
       <c r="B80" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C80" s="85">
+      <c r="C80" s="84">
         <v>0.7</v>
       </c>
-      <c r="D80" s="85">
+      <c r="D80" s="84">
         <v>0.55999999999999994</v>
       </c>
-      <c r="E80" s="85">
+      <c r="E80" s="84">
         <v>0.84</v>
       </c>
       <c r="F80" s="58"/>
       <c r="G80" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="H80" s="88"/>
+      <c r="H80" s="111"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="94"/>
+      <c r="A81" s="99"/>
       <c r="B81" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="C81" s="85">
+      <c r="C81" s="84">
         <v>0.05</v>
       </c>
-      <c r="D81" s="85">
+      <c r="D81" s="84">
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="E81" s="85">
+      <c r="E81" s="84">
         <v>0.06</v>
       </c>
       <c r="F81" s="58"/>
       <c r="G81" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="H81" s="88"/>
+      <c r="H81" s="111"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="94"/>
+      <c r="A82" s="99"/>
       <c r="B82" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="85">
+      <c r="C82" s="84">
         <v>0.05</v>
       </c>
-      <c r="D82" s="85">
+      <c r="D82" s="84">
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="E82" s="85">
+      <c r="E82" s="84">
         <v>0.06</v>
       </c>
       <c r="F82" s="58"/>
       <c r="G82" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="H82" s="89"/>
+      <c r="H82" s="112"/>
     </row>
     <row r="84" spans="1:11">
       <c r="K84" s="13"/>
@@ -4008,33 +4012,33 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="H65:H82"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="H48:H57"/>
+    <mergeCell ref="H61:H64"/>
     <mergeCell ref="A65:A82"/>
     <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A36"/>
-    <mergeCell ref="A49:A64"/>
-    <mergeCell ref="H65:H82"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="H49:H58"/>
-    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="A48:A64"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K36:M36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C52" formula="1"/>
+    <ignoredError sqref="C51" formula="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -4059,13 +4063,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="116" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="4" t="s">
@@ -4091,7 +4095,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -4115,7 +4119,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="96"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4139,11 +4143,11 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="96"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="77">
         <f>ROUNDUP((500/C7),0)</f>
         <v>953</v>
       </c>
@@ -4164,11 +4168,11 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="96"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="77">
         <f>31.5/60</f>
         <v>0.52500000000000002</v>
       </c>
@@ -4189,11 +4193,11 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="96"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="77">
         <v>380</v>
       </c>
       <c r="D8" s="11">
@@ -4210,12 +4214,12 @@
       <c r="G8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H8" s="60" t="s">
+      <c r="H8" s="59" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="96"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -4239,7 +4243,7 @@
       <c r="H9" s="55"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="96"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -4266,11 +4270,11 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="61"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="71"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4283,16 +4287,16 @@
       <c r="G11" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="95" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="61"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4305,14 +4309,14 @@
       <c r="G12" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="114"/>
+      <c r="H12" s="95"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="61"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="71"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4325,14 +4329,14 @@
       <c r="G13" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="114"/>
+      <c r="H13" s="95"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="61"/>
-      <c r="B14" s="70" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="78">
         <v>0.5</v>
       </c>
       <c r="D14" s="40">
@@ -4345,12 +4349,12 @@
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
-      <c r="H14" s="74" t="s">
+      <c r="H14" s="73" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="102" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="47" t="s">
@@ -4374,12 +4378,12 @@
       <c r="G15" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="87" t="s">
+      <c r="H15" s="110" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="98"/>
+      <c r="A16" s="103"/>
       <c r="B16" s="47" t="s">
         <v>74</v>
       </c>
@@ -4401,10 +4405,10 @@
       <c r="G16" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="88"/>
+      <c r="H16" s="111"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="98"/>
+      <c r="A17" s="103"/>
       <c r="B17" s="47" t="s">
         <v>75</v>
       </c>
@@ -4426,10 +4430,10 @@
       <c r="G17" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="89"/>
+      <c r="H17" s="112"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="104" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -4455,7 +4459,7 @@
       <c r="H18" s="50"/>
     </row>
     <row r="19" spans="1:8" ht="28.8">
-      <c r="A19" s="99"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="25" t="s">
         <v>76</v>
       </c>
@@ -4476,12 +4480,12 @@
       <c r="G19" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="77" t="s">
+      <c r="H19" s="76" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="99"/>
+      <c r="A20" s="104"/>
       <c r="B20" s="25" t="s">
         <v>79</v>
       </c>
@@ -4505,7 +4509,7 @@
       <c r="H20" s="50"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="99"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="25" t="s">
         <v>80</v>
       </c>
@@ -4529,7 +4533,7 @@
       <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="99"/>
+      <c r="A22" s="104"/>
       <c r="B22" s="25" t="s">
         <v>86</v>
       </c>
@@ -4553,7 +4557,7 @@
       <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="99"/>
+      <c r="A23" s="104"/>
       <c r="B23" s="25" t="s">
         <v>87</v>
       </c>
@@ -4577,7 +4581,7 @@
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="99"/>
+      <c r="A24" s="104"/>
       <c r="B24" s="25" t="s">
         <v>90</v>
       </c>
@@ -4601,7 +4605,7 @@
       <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="105" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -4625,7 +4629,7 @@
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="101"/>
+      <c r="A26" s="106"/>
       <c r="B26" s="9" t="s">
         <v>12</v>
       </c>
@@ -4647,7 +4651,7 @@
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="101"/>
+      <c r="A27" s="106"/>
       <c r="B27" s="9" t="s">
         <v>13</v>
       </c>
@@ -4669,7 +4673,7 @@
       <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="101"/>
+      <c r="A28" s="106"/>
       <c r="B28" s="9" t="s">
         <v>21</v>
       </c>
@@ -4691,7 +4695,7 @@
       <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="101"/>
+      <c r="A29" s="106"/>
       <c r="B29" s="9" t="s">
         <v>14</v>
       </c>
@@ -4713,7 +4717,7 @@
       <c r="H29" s="50"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="101"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="9" t="s">
         <v>15</v>
       </c>
@@ -4735,7 +4739,7 @@
       <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="101"/>
+      <c r="A31" s="106"/>
       <c r="B31" s="36" t="s">
         <v>16</v>
       </c>
@@ -4759,7 +4763,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="101"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="36" t="s">
         <v>17</v>
       </c>
@@ -4783,11 +4787,11 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="101"/>
+      <c r="A33" s="106"/>
       <c r="B33" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="71"/>
+      <c r="C33" s="70"/>
       <c r="D33" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4800,16 +4804,16 @@
       <c r="G33" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="H33" s="90" t="s">
+      <c r="H33" s="113" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="101"/>
+      <c r="A34" s="106"/>
       <c r="B34" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="71"/>
+      <c r="C34" s="70"/>
       <c r="D34" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4822,14 +4826,14 @@
       <c r="G34" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="91"/>
+      <c r="H34" s="114"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="101"/>
+      <c r="A35" s="106"/>
       <c r="B35" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="71"/>
+      <c r="C35" s="70"/>
       <c r="D35" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4842,14 +4846,14 @@
       <c r="G35" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="H35" s="91"/>
+      <c r="H35" s="114"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="101"/>
+      <c r="A36" s="106"/>
       <c r="B36" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="71"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4862,10 +4866,10 @@
       <c r="G36" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="H36" s="92"/>
+      <c r="H36" s="115"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="111" t="s">
+      <c r="A37" s="92" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="52" t="s">
@@ -4889,12 +4893,12 @@
       <c r="G37" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="H37" s="90" t="s">
+      <c r="H37" s="113" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="112"/>
+      <c r="A38" s="93"/>
       <c r="B38" s="52" t="s">
         <v>27</v>
       </c>
@@ -4916,10 +4920,10 @@
       <c r="G38" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="H38" s="91"/>
+      <c r="H38" s="114"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="112"/>
+      <c r="A39" s="93"/>
       <c r="B39" s="52" t="s">
         <v>28</v>
       </c>
@@ -4941,10 +4945,10 @@
       <c r="G39" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="H39" s="91"/>
+      <c r="H39" s="114"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="112"/>
+      <c r="A40" s="93"/>
       <c r="B40" s="52" t="s">
         <v>29</v>
       </c>
@@ -4966,10 +4970,10 @@
       <c r="G40" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="92"/>
+      <c r="H40" s="115"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="113"/>
+      <c r="A41" s="94"/>
       <c r="B41" s="14" t="s">
         <v>165</v>
       </c>
@@ -4993,7 +4997,7 @@
       <c r="H41" s="50"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="108" t="s">
+      <c r="A42" s="89" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="17" t="s">
@@ -5021,7 +5025,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="109"/>
+      <c r="A43" s="90"/>
       <c r="B43" s="17" t="s">
         <v>33</v>
       </c>
@@ -5045,7 +5049,7 @@
       <c r="H43" s="50"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="109"/>
+      <c r="A44" s="90"/>
       <c r="B44" s="17" t="s">
         <v>34</v>
       </c>
@@ -5071,7 +5075,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="109"/>
+      <c r="A45" s="90"/>
       <c r="B45" s="17" t="s">
         <v>35</v>
       </c>
@@ -5095,7 +5099,7 @@
       <c r="H45" s="50"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="109"/>
+      <c r="A46" s="90"/>
       <c r="B46" s="17" t="s">
         <v>36</v>
       </c>
@@ -5119,7 +5123,7 @@
       <c r="H46" s="50"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="109"/>
+      <c r="A47" s="90"/>
       <c r="B47" s="17" t="s">
         <v>37</v>
       </c>
@@ -5143,7 +5147,7 @@
       <c r="H47" s="50"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="110"/>
+      <c r="A48" s="91"/>
       <c r="B48" s="17" t="s">
         <v>151</v>
       </c>
@@ -5167,7 +5171,7 @@
       <c r="H48" s="50"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="102" t="s">
+      <c r="A49" s="107" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="20" t="s">
@@ -5191,12 +5195,12 @@
       <c r="G49" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="H49" s="90" t="s">
+      <c r="H49" s="113" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="103"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="20" t="s">
         <v>171</v>
       </c>
@@ -5218,14 +5222,14 @@
       <c r="G50" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="H50" s="91"/>
+      <c r="H50" s="114"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="103"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="83">
+      <c r="C51" s="82">
         <f>(9/C56)*0.89</f>
         <v>0.13350000000000001</v>
       </c>
@@ -5243,10 +5247,10 @@
       <c r="G51" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="H51" s="91"/>
+      <c r="H51" s="114"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="103"/>
+      <c r="A52" s="108"/>
       <c r="B52" s="20" t="s">
         <v>225</v>
       </c>
@@ -5268,14 +5272,14 @@
       <c r="G52" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H52" s="91"/>
+      <c r="H52" s="114"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="103"/>
+      <c r="A53" s="108"/>
       <c r="B53" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C53" s="83">
+      <c r="C53" s="82">
         <f>(9/C58)*0.89</f>
         <v>1.3349999999999999E-2</v>
       </c>
@@ -5293,14 +5297,14 @@
       <c r="G53" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="H53" s="91"/>
+      <c r="H53" s="114"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="103"/>
+      <c r="A54" s="108"/>
       <c r="B54" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="C54" s="83">
+      <c r="C54" s="82">
         <f>14.7*60</f>
         <v>882</v>
       </c>
@@ -5318,14 +5322,14 @@
       <c r="G54" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="H54" s="91"/>
+      <c r="H54" s="114"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="103"/>
+      <c r="A55" s="108"/>
       <c r="B55" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C55" s="83">
+      <c r="C55" s="82">
         <v>30</v>
       </c>
       <c r="D55" s="21">
@@ -5342,14 +5346,14 @@
       <c r="G55" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="H55" s="91"/>
+      <c r="H55" s="114"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="103"/>
+      <c r="A56" s="108"/>
       <c r="B56" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C56" s="83">
+      <c r="C56" s="82">
         <v>60</v>
       </c>
       <c r="D56" s="21">
@@ -5366,14 +5370,14 @@
       <c r="G56" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="H56" s="91"/>
+      <c r="H56" s="114"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="103"/>
+      <c r="A57" s="108"/>
       <c r="B57" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C57" s="83">
+      <c r="C57" s="82">
         <f>60*1.0345</f>
         <v>62.07</v>
       </c>
@@ -5391,14 +5395,14 @@
       <c r="G57" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="H57" s="91"/>
+      <c r="H57" s="114"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="103"/>
+      <c r="A58" s="108"/>
       <c r="B58" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="C58" s="83">
+      <c r="C58" s="82">
         <v>600</v>
       </c>
       <c r="D58" s="21">
@@ -5415,10 +5419,10 @@
       <c r="G58" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="H58" s="92"/>
+      <c r="H58" s="115"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="103"/>
+      <c r="A59" s="108"/>
       <c r="B59" s="23" t="s">
         <v>163</v>
       </c>
@@ -5444,7 +5448,7 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="103"/>
+      <c r="A60" s="108"/>
       <c r="B60" s="23" t="s">
         <v>164</v>
       </c>
@@ -5463,12 +5467,12 @@
       <c r="G60" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="H60" s="82" t="s">
+      <c r="H60" s="81" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="103"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="42" t="s">
         <v>41</v>
       </c>
@@ -5490,12 +5494,12 @@
       <c r="G61" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="H61" s="90" t="s">
+      <c r="H61" s="113" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="103"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="42" t="s">
         <v>42</v>
       </c>
@@ -5517,10 +5521,10 @@
       <c r="G62" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="H62" s="91"/>
+      <c r="H62" s="114"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="103"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="42" t="s">
         <v>92</v>
       </c>
@@ -5542,11 +5546,11 @@
       <c r="G63" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="H63" s="91"/>
+      <c r="H63" s="114"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="104"/>
-      <c r="B64" s="73" t="s">
+      <c r="A64" s="109"/>
+      <c r="B64" s="72" t="s">
         <v>93</v>
       </c>
       <c r="C64" s="43">
@@ -5567,263 +5571,263 @@
       <c r="G64" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="H64" s="92"/>
+      <c r="H64" s="115"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="93" t="s">
+      <c r="A65" s="98" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="72"/>
+      <c r="C65" s="71"/>
       <c r="D65" s="57"/>
       <c r="E65" s="57"/>
       <c r="F65" s="58"/>
       <c r="G65" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="H65" s="87" t="s">
+      <c r="H65" s="110" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="94"/>
+      <c r="A66" s="99"/>
       <c r="B66" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="72"/>
+      <c r="C66" s="71"/>
       <c r="D66" s="57"/>
       <c r="E66" s="57"/>
       <c r="F66" s="58"/>
       <c r="G66" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="H66" s="88"/>
+      <c r="H66" s="111"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="94"/>
+      <c r="A67" s="99"/>
       <c r="B67" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C67" s="72"/>
+      <c r="C67" s="71"/>
       <c r="D67" s="57"/>
       <c r="E67" s="57"/>
       <c r="F67" s="58"/>
       <c r="G67" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="H67" s="88"/>
+      <c r="H67" s="111"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="94"/>
+      <c r="A68" s="99"/>
       <c r="B68" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="71"/>
+      <c r="C68" s="70"/>
       <c r="D68" s="57"/>
       <c r="E68" s="57"/>
       <c r="F68" s="58"/>
       <c r="G68" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="H68" s="88"/>
+      <c r="H68" s="111"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="94"/>
+      <c r="A69" s="99"/>
       <c r="B69" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="71"/>
+      <c r="C69" s="70"/>
       <c r="D69" s="57"/>
       <c r="E69" s="57"/>
       <c r="F69" s="58"/>
       <c r="G69" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="H69" s="88"/>
+      <c r="H69" s="111"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="94"/>
+      <c r="A70" s="99"/>
       <c r="B70" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="71"/>
+      <c r="C70" s="70"/>
       <c r="D70" s="57"/>
       <c r="E70" s="57"/>
       <c r="F70" s="58"/>
       <c r="G70" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="88"/>
+      <c r="H70" s="111"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="94"/>
+      <c r="A71" s="99"/>
       <c r="B71" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C71" s="71"/>
+      <c r="C71" s="70"/>
       <c r="D71" s="57"/>
       <c r="E71" s="57"/>
       <c r="F71" s="58"/>
       <c r="G71" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="H71" s="88"/>
+      <c r="H71" s="111"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="94"/>
+      <c r="A72" s="99"/>
       <c r="B72" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="71"/>
+      <c r="C72" s="70"/>
       <c r="D72" s="57"/>
       <c r="E72" s="57"/>
       <c r="F72" s="58"/>
       <c r="G72" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="H72" s="88"/>
+      <c r="H72" s="111"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="94"/>
+      <c r="A73" s="99"/>
       <c r="B73" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C73" s="71"/>
+      <c r="C73" s="70"/>
       <c r="D73" s="57"/>
       <c r="E73" s="57"/>
       <c r="F73" s="58"/>
       <c r="G73" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="H73" s="88"/>
+      <c r="H73" s="111"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="94"/>
+      <c r="A74" s="99"/>
       <c r="B74" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C74" s="71"/>
+      <c r="C74" s="70"/>
       <c r="D74" s="57"/>
       <c r="E74" s="57"/>
       <c r="F74" s="58"/>
       <c r="G74" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H74" s="88"/>
+      <c r="H74" s="111"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="94"/>
+      <c r="A75" s="99"/>
       <c r="B75" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="71"/>
+      <c r="C75" s="70"/>
       <c r="D75" s="57"/>
       <c r="E75" s="57"/>
       <c r="F75" s="58"/>
       <c r="G75" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="H75" s="88"/>
+      <c r="H75" s="111"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="94"/>
+      <c r="A76" s="99"/>
       <c r="B76" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C76" s="71"/>
+      <c r="C76" s="70"/>
       <c r="D76" s="57"/>
       <c r="E76" s="57"/>
       <c r="F76" s="58"/>
       <c r="G76" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="H76" s="88"/>
+      <c r="H76" s="111"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="94"/>
+      <c r="A77" s="99"/>
       <c r="B77" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C77" s="71"/>
+      <c r="C77" s="70"/>
       <c r="D77" s="57"/>
       <c r="E77" s="57"/>
       <c r="F77" s="58"/>
       <c r="G77" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="H77" s="88"/>
+      <c r="H77" s="111"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="94"/>
+      <c r="A78" s="99"/>
       <c r="B78" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C78" s="72"/>
+      <c r="C78" s="71"/>
       <c r="D78" s="57"/>
       <c r="E78" s="57"/>
       <c r="F78" s="58"/>
       <c r="G78" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="H78" s="88"/>
+      <c r="H78" s="111"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="94"/>
+      <c r="A79" s="99"/>
       <c r="B79" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C79" s="72"/>
+      <c r="C79" s="71"/>
       <c r="D79" s="57"/>
       <c r="E79" s="57"/>
       <c r="F79" s="58"/>
       <c r="G79" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H79" s="88"/>
+      <c r="H79" s="111"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="94"/>
+      <c r="A80" s="99"/>
       <c r="B80" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C80" s="72"/>
+      <c r="C80" s="71"/>
       <c r="D80" s="57"/>
       <c r="E80" s="57"/>
       <c r="F80" s="58"/>
       <c r="G80" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="H80" s="88"/>
+      <c r="H80" s="111"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="94"/>
+      <c r="A81" s="99"/>
       <c r="B81" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="C81" s="72"/>
+      <c r="C81" s="71"/>
       <c r="D81" s="57"/>
       <c r="E81" s="57"/>
       <c r="F81" s="58"/>
       <c r="G81" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="H81" s="88"/>
+      <c r="H81" s="111"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="94"/>
+      <c r="A82" s="99"/>
       <c r="B82" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="72"/>
+      <c r="C82" s="71"/>
       <c r="D82" s="57"/>
       <c r="E82" s="57"/>
       <c r="F82" s="58"/>
       <c r="G82" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="H82" s="89"/>
+      <c r="H82" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5854,6 +5858,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D2CC3865CED4124A9830BAAA78333A39" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="74fbc97153726fbf9f4b2acfe0ba4f2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="47151ffa-27c1-491d-bdc5-fff6d8a44614" xmlns:ns4="2a729546-cf4e-435c-aabc-21366d2421e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef40a5df47e7cf58b55af26490b848e0" ns3:_="" ns4:_="">
     <xsd:import namespace="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
@@ -6076,12 +6086,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6092,6 +6096,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145C285F-2FF3-4D38-95ED-9BA60F4E3C89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D48284-4FE0-49DC-82DA-D80B72208958}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6110,23 +6131,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145C285F-2FF3-4D38-95ED-9BA60F4E3C89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9031FEDD-5FF8-4C9C-AF51-AEFA4BF396D5}">
   <ds:schemaRefs>

</xml_diff>